<commit_message>
inverse availability, support dates, support results upload
</commit_message>
<xml_diff>
--- a/test_data/lect_and_guide/Calendar_for_2023.xlsx
+++ b/test_data/lect_and_guide/Calendar_for_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\travkaie\PycharmProjects\LogisticModel\test_data\_data_no_index\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\travkaie\PycharmProjects\LogisticModel\test_data\lect_and_guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF96914-80AA-4317-B2F8-0CE4C3BE9D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014238CE-AEEC-4D77-AC1F-4CF7695D85BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="פנינה יעקב" sheetId="20" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92FDE9E-B7A4-4FD2-A01D-2BDAAEB5CEED}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -534,11 +534,11 @@
           </x14:formula1>
           <xm:sqref>A2:A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{068BB0DC-F126-4088-A37A-55696EEF3A43}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9B6B6D2-75BF-4882-BCA8-9E5EE6B1618E}">
           <x14:formula1>
-            <xm:f>Slots!$F$3</xm:f>
+            <xm:f>Slots!$F$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
+          <xm:sqref>B2:B508</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -551,7 +551,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>